<commit_message>
add thunder bay spawning dates
</commit_message>
<xml_diff>
--- a/data/lake-superior-apostle-islands/lake-superior-apostle-islands-spawning.xlsx
+++ b/data/lake-superior-apostle-islands/lake-superior-apostle-islands-spawning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-DegreeDay-Modeling/data/lake-superior-apostle-islands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148C6C55-14AB-1847-BB84-ECB981481AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C09CCF9-78B5-7A4D-B1AA-F711BCDA8524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="12520" windowHeight="19200" xr2:uid="{6BC05E8D-020F-47A5-B927-8B963608FB42}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>month</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>spent</t>
+  </si>
+  <si>
+    <t>prop.ripe</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D229DAE8-BA4F-4710-8890-5ECB8E562013}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -441,7 +444,7 @@
     <col min="4" max="4" width="13.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -463,8 +466,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42340</v>
       </c>
@@ -488,8 +494,12 @@
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <f>F2/SUM(E2:G2)</f>
+        <v>6.1728395061728392E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42345</v>
       </c>
@@ -513,8 +523,12 @@
       <c r="G3">
         <v>3</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="2">F3/SUM(E3:G3)</f>
+        <v>9.4017094017094016E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>42705</v>
       </c>
@@ -538,8 +552,12 @@
       <c r="G4">
         <v>0</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>2.9850746268656716E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>42706</v>
       </c>
@@ -563,8 +581,12 @@
       <c r="G5">
         <v>0</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42710</v>
       </c>
@@ -588,8 +610,12 @@
       <c r="G6">
         <v>0</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43079</v>
       </c>
@@ -612,6 +638,10 @@
       </c>
       <c r="G7">
         <v>16</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>0.11627906976744186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>